<commit_message>
Player Skill NormalAttackUp 추가
</commit_message>
<xml_diff>
--- a/Assets/Resources/StaticData/Excel/PlayerActiveSkills.xlsx
+++ b/Assets/Resources/StaticData/Excel/PlayerActiveSkills.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\CoffeeCat_RogueLite_Project\Assets\StaticData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\CoffeeCat_RogueLite_Project\Assets\Resources\StaticData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF231727-D17B-41D9-BCCA-07C87B059103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ABAD66-1597-4791-B6FC-E221F261DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CEFF60A8-3F85-4A92-8727-6613D870E2B7}"/>
+    <workbookView xWindow="-16320" yWindow="-6870" windowWidth="16440" windowHeight="28320" xr2:uid="{CEFF60A8-3F85-4A92-8727-6613D870E2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFB7CDA-B6DD-480D-906E-C7E484E83C4A}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -550,15 +550,14 @@
     <col min="7" max="7" width="14.25" customWidth="1"/>
     <col min="8" max="8" width="17.25" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="14.125" customWidth="1"/>
-    <col min="11" max="11" width="16.75" customWidth="1"/>
-    <col min="12" max="12" width="14.25" customWidth="1"/>
-    <col min="13" max="13" width="16.75" customWidth="1"/>
-    <col min="14" max="16" width="19.75" customWidth="1"/>
-    <col min="17" max="17" width="13.125" customWidth="1"/>
+    <col min="10" max="10" width="16.75" customWidth="1"/>
+    <col min="11" max="11" width="14.25" customWidth="1"/>
+    <col min="12" max="12" width="16.75" customWidth="1"/>
+    <col min="13" max="15" width="19.75" customWidth="1"/>
+    <col min="16" max="16" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -593,9 +592,8 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -630,9 +628,8 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -667,9 +664,8 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -704,9 +700,8 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -735,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -764,7 +759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -793,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -822,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -851,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -879,6 +874,17 @@
       <c r="I10" s="2">
         <v>1</v>
       </c>
+    </row>
+    <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>